<commit_message>
updated hours of sleep
</commit_message>
<xml_diff>
--- a/Design Data/Sample Data/Excel Files/Water Intake.xlsx
+++ b/Design Data/Sample Data/Excel Files/Water Intake.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S538408\Documents\GDP\gdp_health_app\Design Data\Sample Data\Excel Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EDAEBE9-DFCC-40E9-9201-A400AB726356}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD323EA5-6813-496C-814D-7AE571D7DA7D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Water Intake" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="32">
   <si>
     <t>3.7 liters</t>
   </si>
@@ -83,13 +83,52 @@
   </si>
   <si>
     <t>User ID</t>
+  </si>
+  <si>
+    <t>Hours of sleep(8 hours)</t>
+  </si>
+  <si>
+    <t>7.5 hours</t>
+  </si>
+  <si>
+    <t>7.7 hours</t>
+  </si>
+  <si>
+    <t>7.2 hours</t>
+  </si>
+  <si>
+    <t>8 hours</t>
+  </si>
+  <si>
+    <t>7 hours</t>
+  </si>
+  <si>
+    <t>9 hours</t>
+  </si>
+  <si>
+    <t>7.9 hours</t>
+  </si>
+  <si>
+    <t>8.1 hours</t>
+  </si>
+  <si>
+    <t>7.8 hours</t>
+  </si>
+  <si>
+    <t>6.5 hours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.5 hours </t>
+  </si>
+  <si>
+    <t>7.1 hours</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,6 +149,12 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -132,7 +177,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -149,6 +194,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -431,8 +477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1280,17 +1326,846 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E55C12AA-C1A9-4DF4-80D0-E236B821A795}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:Q16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.81640625" customWidth="1"/>
+    <col min="1" max="1" width="8.54296875" customWidth="1"/>
+    <col min="2" max="2" width="10.26953125" customWidth="1"/>
+    <col min="11" max="11" width="9.453125" customWidth="1"/>
+    <col min="12" max="12" width="9.36328125" customWidth="1"/>
+    <col min="13" max="13" width="9.453125" customWidth="1"/>
+    <col min="14" max="14" width="9.54296875" customWidth="1"/>
+    <col min="15" max="15" width="9.7265625" customWidth="1"/>
+    <col min="16" max="16" width="9.90625" customWidth="1"/>
+    <col min="17" max="17" width="9.453125" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="3">
+        <v>44075</v>
+      </c>
+      <c r="C2" s="3">
+        <v>44076</v>
+      </c>
+      <c r="D2" s="3">
+        <v>44077</v>
+      </c>
+      <c r="E2" s="3">
+        <v>44078</v>
+      </c>
+      <c r="F2" s="3">
+        <v>44079</v>
+      </c>
+      <c r="G2" s="3">
+        <v>44080</v>
+      </c>
+      <c r="H2" s="3">
+        <v>44081</v>
+      </c>
+      <c r="I2" s="3">
+        <v>44082</v>
+      </c>
+      <c r="J2" s="3">
+        <v>44083</v>
+      </c>
+      <c r="K2" s="3">
+        <v>44084</v>
+      </c>
+      <c r="L2" s="3">
+        <v>44085</v>
+      </c>
+      <c r="M2" s="3">
+        <v>44086</v>
+      </c>
+      <c r="N2" s="3">
+        <v>44087</v>
+      </c>
+      <c r="O2" s="3">
+        <v>44088</v>
+      </c>
+      <c r="P2" s="3">
+        <v>44089</v>
+      </c>
+      <c r="Q2" s="3">
+        <v>44090</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A3" s="4">
+        <v>101</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O3" t="s">
+        <v>21</v>
+      </c>
+      <c r="P3" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A4" s="4">
+        <v>102</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4" t="s">
+        <v>20</v>
+      </c>
+      <c r="L4" t="s">
+        <v>22</v>
+      </c>
+      <c r="M4" t="s">
+        <v>23</v>
+      </c>
+      <c r="N4" t="s">
+        <v>20</v>
+      </c>
+      <c r="O4" t="s">
+        <v>25</v>
+      </c>
+      <c r="P4" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A5" s="4">
+        <v>103</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K5" t="s">
+        <v>20</v>
+      </c>
+      <c r="L5" t="s">
+        <v>21</v>
+      </c>
+      <c r="M5" t="s">
+        <v>22</v>
+      </c>
+      <c r="N5" t="s">
+        <v>23</v>
+      </c>
+      <c r="O5" t="s">
+        <v>23</v>
+      </c>
+      <c r="P5" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A6" s="4">
+        <v>104</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J6" t="s">
+        <v>24</v>
+      </c>
+      <c r="K6" t="s">
+        <v>24</v>
+      </c>
+      <c r="L6" t="s">
+        <v>24</v>
+      </c>
+      <c r="M6" t="s">
+        <v>24</v>
+      </c>
+      <c r="N6" t="s">
+        <v>24</v>
+      </c>
+      <c r="O6" t="s">
+        <v>24</v>
+      </c>
+      <c r="P6" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A7" s="4">
+        <v>105</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" t="s">
+        <v>28</v>
+      </c>
+      <c r="H7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J7" t="s">
+        <v>20</v>
+      </c>
+      <c r="K7" t="s">
+        <v>28</v>
+      </c>
+      <c r="L7" t="s">
+        <v>20</v>
+      </c>
+      <c r="M7" t="s">
+        <v>28</v>
+      </c>
+      <c r="N7" t="s">
+        <v>20</v>
+      </c>
+      <c r="O7" t="s">
+        <v>28</v>
+      </c>
+      <c r="P7" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A8" s="4">
+        <v>106</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I8" t="s">
+        <v>23</v>
+      </c>
+      <c r="J8" t="s">
+        <v>23</v>
+      </c>
+      <c r="K8" t="s">
+        <v>23</v>
+      </c>
+      <c r="L8" t="s">
+        <v>23</v>
+      </c>
+      <c r="M8" t="s">
+        <v>23</v>
+      </c>
+      <c r="N8" t="s">
+        <v>23</v>
+      </c>
+      <c r="O8" t="s">
+        <v>23</v>
+      </c>
+      <c r="P8" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A9" s="4">
+        <v>107</v>
+      </c>
+      <c r="B9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" t="s">
+        <v>25</v>
+      </c>
+      <c r="I9" t="s">
+        <v>23</v>
+      </c>
+      <c r="J9" t="s">
+        <v>23</v>
+      </c>
+      <c r="K9" t="s">
+        <v>23</v>
+      </c>
+      <c r="L9" t="s">
+        <v>23</v>
+      </c>
+      <c r="M9" t="s">
+        <v>30</v>
+      </c>
+      <c r="N9" t="s">
+        <v>31</v>
+      </c>
+      <c r="O9" t="s">
+        <v>25</v>
+      </c>
+      <c r="P9" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A10" s="4">
+        <v>108</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" t="s">
+        <v>20</v>
+      </c>
+      <c r="I10" t="s">
+        <v>22</v>
+      </c>
+      <c r="J10" t="s">
+        <v>23</v>
+      </c>
+      <c r="K10" t="s">
+        <v>23</v>
+      </c>
+      <c r="L10" t="s">
+        <v>22</v>
+      </c>
+      <c r="M10" t="s">
+        <v>22</v>
+      </c>
+      <c r="N10" t="s">
+        <v>20</v>
+      </c>
+      <c r="O10" t="s">
+        <v>21</v>
+      </c>
+      <c r="P10" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A11" s="4">
+        <v>109</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" t="s">
+        <v>27</v>
+      </c>
+      <c r="H11" t="s">
+        <v>20</v>
+      </c>
+      <c r="I11" t="s">
+        <v>22</v>
+      </c>
+      <c r="J11" t="s">
+        <v>20</v>
+      </c>
+      <c r="K11" t="s">
+        <v>20</v>
+      </c>
+      <c r="L11" t="s">
+        <v>25</v>
+      </c>
+      <c r="M11" t="s">
+        <v>20</v>
+      </c>
+      <c r="N11" t="s">
+        <v>26</v>
+      </c>
+      <c r="O11" t="s">
+        <v>20</v>
+      </c>
+      <c r="P11" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A12" s="4">
+        <v>110</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" t="s">
+        <v>23</v>
+      </c>
+      <c r="H12" t="s">
+        <v>23</v>
+      </c>
+      <c r="I12" t="s">
+        <v>23</v>
+      </c>
+      <c r="J12" t="s">
+        <v>23</v>
+      </c>
+      <c r="K12" t="s">
+        <v>23</v>
+      </c>
+      <c r="L12" t="s">
+        <v>23</v>
+      </c>
+      <c r="M12" t="s">
+        <v>23</v>
+      </c>
+      <c r="N12" t="s">
+        <v>23</v>
+      </c>
+      <c r="O12" t="s">
+        <v>23</v>
+      </c>
+      <c r="P12" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A13" s="4">
+        <v>111</v>
+      </c>
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" t="s">
+        <v>20</v>
+      </c>
+      <c r="H13" t="s">
+        <v>20</v>
+      </c>
+      <c r="I13" t="s">
+        <v>20</v>
+      </c>
+      <c r="J13" t="s">
+        <v>20</v>
+      </c>
+      <c r="K13" t="s">
+        <v>20</v>
+      </c>
+      <c r="L13" t="s">
+        <v>20</v>
+      </c>
+      <c r="M13" t="s">
+        <v>20</v>
+      </c>
+      <c r="N13" t="s">
+        <v>20</v>
+      </c>
+      <c r="O13" t="s">
+        <v>20</v>
+      </c>
+      <c r="P13" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A14" s="4">
+        <v>112</v>
+      </c>
+      <c r="B14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" t="s">
+        <v>23</v>
+      </c>
+      <c r="G14" t="s">
+        <v>22</v>
+      </c>
+      <c r="H14" t="s">
+        <v>22</v>
+      </c>
+      <c r="I14" t="s">
+        <v>20</v>
+      </c>
+      <c r="J14" t="s">
+        <v>21</v>
+      </c>
+      <c r="K14" t="s">
+        <v>22</v>
+      </c>
+      <c r="L14" t="s">
+        <v>22</v>
+      </c>
+      <c r="M14" t="s">
+        <v>20</v>
+      </c>
+      <c r="N14" t="s">
+        <v>22</v>
+      </c>
+      <c r="O14" t="s">
+        <v>23</v>
+      </c>
+      <c r="P14" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A15" s="4">
+        <v>113</v>
+      </c>
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F15" t="s">
+        <v>20</v>
+      </c>
+      <c r="G15" t="s">
+        <v>22</v>
+      </c>
+      <c r="H15" t="s">
+        <v>20</v>
+      </c>
+      <c r="I15" t="s">
+        <v>22</v>
+      </c>
+      <c r="J15" t="s">
+        <v>23</v>
+      </c>
+      <c r="K15" t="s">
+        <v>20</v>
+      </c>
+      <c r="L15" t="s">
+        <v>25</v>
+      </c>
+      <c r="M15" t="s">
+        <v>20</v>
+      </c>
+      <c r="N15" t="s">
+        <v>23</v>
+      </c>
+      <c r="O15" t="s">
+        <v>20</v>
+      </c>
+      <c r="P15" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A16" s="4">
+        <v>114</v>
+      </c>
+      <c r="B16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" t="s">
+        <v>22</v>
+      </c>
+      <c r="F16" t="s">
+        <v>23</v>
+      </c>
+      <c r="G16" t="s">
+        <v>23</v>
+      </c>
+      <c r="H16" t="s">
+        <v>23</v>
+      </c>
+      <c r="I16" t="s">
+        <v>23</v>
+      </c>
+      <c r="J16" t="s">
+        <v>23</v>
+      </c>
+      <c r="K16" t="s">
+        <v>23</v>
+      </c>
+      <c r="L16" t="s">
+        <v>23</v>
+      </c>
+      <c r="M16" t="s">
+        <v>20</v>
+      </c>
+      <c r="N16" t="s">
+        <v>20</v>
+      </c>
+      <c r="O16" t="s">
+        <v>20</v>
+      </c>
+      <c r="P16" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:Q1"/>
+  </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>